<commit_message>
moved all parameter to the excel sheet, added code to compute table for zero andpusher k_eq
</commit_message>
<xml_diff>
--- a/Settings.xlsx
+++ b/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathann\ClawdDrive\Code\FlexProbeOptimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2EBEF3-95B0-4199-A496-5B74049BD5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE31410-34E3-4863-87DB-8028EB338B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11033" yWindow="1673" windowWidth="10942" windowHeight="13679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="577" yWindow="0" windowWidth="16051" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>mm</t>
   </si>
@@ -52,6 +52,57 @@
   </si>
   <si>
     <t>bladeThicknessZeroConverter</t>
+  </si>
+  <si>
+    <t>forceMinRigidity</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>forceMaxRigidity</t>
+  </si>
+  <si>
+    <t>rangeXProbeMax</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>rangeXProbeMin</t>
+  </si>
+  <si>
+    <t>Eyoung</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>bladeLengthZeroConverter</t>
+  </si>
+  <si>
+    <t>bladeLengthForceConverter</t>
+  </si>
+  <si>
+    <t>bladeLengthWheelAnchor</t>
+  </si>
+  <si>
+    <t>BladeLengthRCC</t>
+  </si>
+  <si>
+    <t>bladeLengthTable</t>
+  </si>
+  <si>
+    <t>bladeLengthTablePushing</t>
+  </si>
+  <si>
+    <t>RCCdeadCenter</t>
+  </si>
+  <si>
+    <t>thicknessWheelPlate</t>
+  </si>
+  <si>
+    <t>thicknessConverterPlate</t>
   </si>
 </sst>
 </file>
@@ -369,15 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26.06640625" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -407,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -426,7 +478,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.1</v>
@@ -437,10 +489,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>-1.85</v>
+        <v>0.1</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -448,23 +500,177 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>0.1</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>2.65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>110000000000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>7.5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>12.125</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>11.98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0.1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>-1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>0.3</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all is computed right excpet non linéarity
</commit_message>
<xml_diff>
--- a/Settings.xlsx
+++ b/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathann\ClawdDrive\Code\FlexProbeOptimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE31410-34E3-4863-87DB-8028EB338B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5A04FD-E9F5-4A1B-99CE-A333270D15E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="577" yWindow="0" windowWidth="16051" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12285" yWindow="795" windowWidth="16050" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2.5299999999999998</v>
+        <v>2.63</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -514,7 +514,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>2.65</v>
+        <v>1.3149999999999999</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>

</xml_diff>